<commit_message>
Runnin all 3 sites, all data, new water and root model. But results unstable.
</commit_message>
<xml_diff>
--- a/model/LERG Notes.xlsx
+++ b/model/LERG Notes.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Simon\Projects\Tiller_Persistence\basgra_nz\model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WoodwardS\Documents\Projects\Tiller_Persistence\basgra_nz\model\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1590" yWindow="0" windowWidth="28800" windowHeight="12795"/>
+    <workbookView xWindow="4680" yWindow="0" windowWidth="28800" windowHeight="12795"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="171027" iterate="1" iterateCount="5000" iterateDelta="0.01" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t xml:space="preserve"> LERV   =          max(0., (-0.76 + 0.52*EFFTMP)/1000. ) ! m d-1 leaf elongation rate on vegetative tillers</t>
   </si>
@@ -39,6 +39,15 @@
   </si>
   <si>
     <t>LERG</t>
+  </si>
+  <si>
+    <t>ratio</t>
+  </si>
+  <si>
+    <t>PeacockLERG</t>
+  </si>
+  <si>
+    <t>ratioP</t>
   </si>
 </sst>
 </file>
@@ -542,6 +551,207 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-A91E-4AD2-9153-A83F00C7C501}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>PeacockLERG</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$7:$D$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>22</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$G$7:$G$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.790000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.4500000000000008E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.1100000000000009E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.7700000000000009E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.2430000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.5090000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.7749999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.0410000000000005E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.307E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.5730000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.8390000000000009E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.1050000000000005E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.3710000000000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.6370000000000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.9030000000000009E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4.1690000000000005E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4.4350000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>4.7010000000000003E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C459-4254-96B1-EA498962082A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1644,25 +1854,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:F29"/>
+  <dimension ref="C3:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X25" sqref="X25"/>
+      <selection activeCell="X21" sqref="X21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
         <v>2</v>
       </c>
@@ -1672,8 +1882,17 @@
       <c r="F6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D7">
         <v>0</v>
       </c>
@@ -1685,8 +1904,20 @@
         <f xml:space="preserve">  MAX(0, (-5.46 + 2.8*D7)/1000 )</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G7">
+        <f xml:space="preserve">  MAX(0, (-11.51 + 2.66*D7)/1000 )</f>
+        <v>0</v>
+      </c>
+      <c r="H7" t="e">
+        <f>F7/E7</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I7" t="e">
+        <f>G7/E7</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="8" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D8">
         <f>D7+1</f>
         <v>1</v>
@@ -1699,10 +1930,22 @@
         <f t="shared" ref="F8:F29" si="1" xml:space="preserve">  MAX(0, (-5.46 + 2.8*D8)/1000 )</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G8">
+        <f t="shared" ref="G8:G29" si="2" xml:space="preserve">  MAX(0, (-11.51 + 2.66*D8)/1000 )</f>
+        <v>0</v>
+      </c>
+      <c r="H8" t="e">
+        <f>F8/E8</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I8" t="e">
+        <f t="shared" ref="I8:I29" si="3">G8/E8</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="9" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D9">
-        <f t="shared" ref="D9:D29" si="2">D8+1</f>
+        <f t="shared" ref="D9:D29" si="4">D8+1</f>
         <v>2</v>
       </c>
       <c r="E9">
@@ -1713,10 +1956,22 @@
         <f t="shared" si="1"/>
         <v>1.3999999999999969E-4</v>
       </c>
-    </row>
-    <row r="10" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <f>F9/E9</f>
+        <v>0.49999999999999883</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="E10">
@@ -1727,10 +1982,22 @@
         <f t="shared" si="1"/>
         <v>2.9399999999999986E-3</v>
       </c>
-    </row>
-    <row r="11" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <f>F10/E10</f>
+        <v>3.674999999999998</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="E11">
@@ -1741,10 +2008,22 @@
         <f t="shared" si="1"/>
         <v>5.7399999999999994E-3</v>
       </c>
-    </row>
-    <row r="12" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <f>F11/E11</f>
+        <v>4.3484848484848477</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="E12">
@@ -1755,10 +2034,22 @@
         <f t="shared" si="1"/>
         <v>8.539999999999999E-3</v>
       </c>
-    </row>
-    <row r="13" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G12">
+        <f t="shared" si="2"/>
+        <v>1.790000000000001E-3</v>
+      </c>
+      <c r="H12">
+        <f>F12/E12</f>
+        <v>4.641304347826086</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="3"/>
+        <v>0.97282608695652228</v>
+      </c>
+    </row>
+    <row r="13" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="E13">
@@ -1769,10 +2060,22 @@
         <f t="shared" si="1"/>
         <v>1.1339999999999996E-2</v>
       </c>
-    </row>
-    <row r="14" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G13">
+        <f t="shared" si="2"/>
+        <v>4.4500000000000008E-3</v>
+      </c>
+      <c r="H13">
+        <f>F13/E13</f>
+        <v>4.8050847457627102</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="3"/>
+        <v>1.8855932203389834</v>
+      </c>
+    </row>
+    <row r="14" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="E14">
@@ -1783,10 +2086,22 @@
         <f t="shared" si="1"/>
         <v>1.4139999999999996E-2</v>
       </c>
-    </row>
-    <row r="15" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G14">
+        <f t="shared" si="2"/>
+        <v>7.1100000000000009E-3</v>
+      </c>
+      <c r="H14">
+        <f>F14/E14</f>
+        <v>4.9097222222222214</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="3"/>
+        <v>2.4687500000000004</v>
+      </c>
+    </row>
+    <row r="15" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="E15">
@@ -1797,10 +2112,22 @@
         <f t="shared" si="1"/>
         <v>1.6939999999999997E-2</v>
       </c>
-    </row>
-    <row r="16" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G15">
+        <f t="shared" si="2"/>
+        <v>9.7700000000000009E-3</v>
+      </c>
+      <c r="H15">
+        <f>F15/E15</f>
+        <v>4.9823529411764689</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="3"/>
+        <v>2.8735294117647059</v>
+      </c>
+    </row>
+    <row r="16" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>9</v>
       </c>
       <c r="E16">
@@ -1811,10 +2138,22 @@
         <f t="shared" si="1"/>
         <v>1.9739999999999997E-2</v>
       </c>
-    </row>
-    <row r="17" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="G16">
+        <f t="shared" si="2"/>
+        <v>1.2430000000000002E-2</v>
+      </c>
+      <c r="H16">
+        <f>F16/E16</f>
+        <v>5.0357142857142856</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="3"/>
+        <v>3.1709183673469394</v>
+      </c>
+    </row>
+    <row r="17" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="E17">
@@ -1825,10 +2164,22 @@
         <f t="shared" si="1"/>
         <v>2.2539999999999998E-2</v>
       </c>
-    </row>
-    <row r="18" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="G17">
+        <f t="shared" si="2"/>
+        <v>1.5090000000000001E-2</v>
+      </c>
+      <c r="H17">
+        <f>F17/E17</f>
+        <v>5.076576576576576</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="3"/>
+        <v>3.3986486486486487</v>
+      </c>
+    </row>
+    <row r="18" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
       <c r="E18">
@@ -1839,10 +2190,22 @@
         <f t="shared" si="1"/>
         <v>2.5339999999999998E-2</v>
       </c>
-    </row>
-    <row r="19" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="G18">
+        <f t="shared" si="2"/>
+        <v>1.7749999999999998E-2</v>
+      </c>
+      <c r="H18">
+        <f>F18/E18</f>
+        <v>5.1088709677419342</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="3"/>
+        <v>3.5786290322580636</v>
+      </c>
+    </row>
+    <row r="19" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
       <c r="E19">
@@ -1853,10 +2216,22 @@
         <f t="shared" si="1"/>
         <v>2.8139999999999995E-2</v>
       </c>
-    </row>
-    <row r="20" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="G19">
+        <f t="shared" si="2"/>
+        <v>2.0410000000000005E-2</v>
+      </c>
+      <c r="H19">
+        <f>F19/E19</f>
+        <v>5.1350364963503639</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="3"/>
+        <v>3.7244525547445262</v>
+      </c>
+    </row>
+    <row r="20" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>13</v>
       </c>
       <c r="E20">
@@ -1867,10 +2242,22 @@
         <f t="shared" si="1"/>
         <v>3.0939999999999999E-2</v>
       </c>
-    </row>
-    <row r="21" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="G20">
+        <f t="shared" si="2"/>
+        <v>2.307E-2</v>
+      </c>
+      <c r="H20">
+        <f>F20/E20</f>
+        <v>5.1566666666666663</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="3"/>
+        <v>3.8449999999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="E21">
@@ -1881,10 +2268,22 @@
         <f t="shared" si="1"/>
         <v>3.3739999999999992E-2</v>
       </c>
-    </row>
-    <row r="22" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="G21">
+        <f t="shared" si="2"/>
+        <v>2.5730000000000003E-2</v>
+      </c>
+      <c r="H21">
+        <f>F21/E21</f>
+        <v>5.174846625766869</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="3"/>
+        <v>3.9463190184049082</v>
+      </c>
+    </row>
+    <row r="22" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
       <c r="E22">
@@ -1895,10 +2294,22 @@
         <f t="shared" si="1"/>
         <v>3.6539999999999996E-2</v>
       </c>
-    </row>
-    <row r="23" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="G22">
+        <f t="shared" si="2"/>
+        <v>2.8390000000000009E-2</v>
+      </c>
+      <c r="H22">
+        <f>F22/E22</f>
+        <v>5.1903409090909074</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="3"/>
+        <v>4.032670454545455</v>
+      </c>
+    </row>
+    <row r="23" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
       <c r="E23">
@@ -1909,10 +2320,22 @@
         <f t="shared" si="1"/>
         <v>3.9339999999999993E-2</v>
       </c>
-    </row>
-    <row r="24" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="G23">
+        <f t="shared" si="2"/>
+        <v>3.1050000000000005E-2</v>
+      </c>
+      <c r="H23">
+        <f>F23/E23</f>
+        <v>5.2037037037037024</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="3"/>
+        <v>4.1071428571428577</v>
+      </c>
+    </row>
+    <row r="24" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>17</v>
       </c>
       <c r="E24">
@@ -1923,10 +2346,22 @@
         <f t="shared" si="1"/>
         <v>4.2139999999999997E-2</v>
       </c>
-    </row>
-    <row r="25" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="G24">
+        <f t="shared" si="2"/>
+        <v>3.3710000000000004E-2</v>
+      </c>
+      <c r="H24">
+        <f>F24/E24</f>
+        <v>5.2153465346534649</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="3"/>
+        <v>4.1720297029702973</v>
+      </c>
+    </row>
+    <row r="25" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
       <c r="E25">
@@ -1937,10 +2372,22 @@
         <f t="shared" si="1"/>
         <v>4.4940000000000001E-2</v>
       </c>
-    </row>
-    <row r="26" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="G25">
+        <f t="shared" si="2"/>
+        <v>3.6370000000000006E-2</v>
+      </c>
+      <c r="H25">
+        <f>F25/E25</f>
+        <v>5.2255813953488373</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="3"/>
+        <v>4.2290697674418611</v>
+      </c>
+    </row>
+    <row r="26" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>19</v>
       </c>
       <c r="E26">
@@ -1951,10 +2398,22 @@
         <f t="shared" si="1"/>
         <v>4.7739999999999998E-2</v>
       </c>
-    </row>
-    <row r="27" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="G26">
+        <f t="shared" si="2"/>
+        <v>3.9030000000000009E-2</v>
+      </c>
+      <c r="H26">
+        <f>F26/E26</f>
+        <v>5.2346491228070162</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="3"/>
+        <v>4.2796052631578947</v>
+      </c>
+    </row>
+    <row r="27" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
       <c r="E27">
@@ -1965,10 +2424,22 @@
         <f t="shared" si="1"/>
         <v>5.0540000000000002E-2</v>
       </c>
-    </row>
-    <row r="28" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="G27">
+        <f t="shared" si="2"/>
+        <v>4.1690000000000005E-2</v>
+      </c>
+      <c r="H27">
+        <f>F27/E27</f>
+        <v>5.2427385892116183</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="3"/>
+        <v>4.3246887966804977</v>
+      </c>
+    </row>
+    <row r="28" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>21</v>
       </c>
       <c r="E28">
@@ -1979,10 +2450,22 @@
         <f t="shared" si="1"/>
         <v>5.3339999999999999E-2</v>
       </c>
-    </row>
-    <row r="29" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="G28">
+        <f t="shared" si="2"/>
+        <v>4.4350000000000001E-2</v>
+      </c>
+      <c r="H28">
+        <f>F28/E28</f>
+        <v>5.2499999999999991</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="3"/>
+        <v>4.3651574803149602</v>
+      </c>
+    </row>
+    <row r="29" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>22</v>
       </c>
       <c r="E29">
@@ -1992,6 +2475,18 @@
       <c r="F29">
         <f t="shared" si="1"/>
         <v>5.6139999999999995E-2</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="2"/>
+        <v>4.7010000000000003E-2</v>
+      </c>
+      <c r="H29">
+        <f>F29/E29</f>
+        <v>5.2565543071161036</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="3"/>
+        <v>4.4016853932584263</v>
       </c>
     </row>
   </sheetData>

</xml_diff>